<commit_message>
clean up master timeline
</commit_message>
<xml_diff>
--- a/Caribbean/master_timeline.xlsx
+++ b/Caribbean/master_timeline.xlsx
@@ -1983,10 +1983,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="str">
-        <f>sheetnam</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>

</xml_diff>